<commit_message>
updated spreadsheets from sampling 8/11
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706C735D-F544-41D1-9B9A-D59E1A00651C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4E184-44C9-4FE0-A9DA-5167BAB4BD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,6 +936,17 @@
         <v>26.2</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44054.365972222222</v>
+      </c>
+      <c r="B4">
+        <v>46.46</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -946,7 +957,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,6 +1314,17 @@
         <v>26.2</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.487500000003</v>
+      </c>
+      <c r="B17">
+        <v>15.52</v>
+      </c>
+      <c r="C17">
+        <v>24.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1311,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,6 +1522,17 @@
         <v>24.8</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.505555555559</v>
+      </c>
+      <c r="B17">
+        <v>51.96</v>
+      </c>
+      <c r="C17">
+        <v>22.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1507,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,6 +1729,17 @@
         <v>25.1</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.390972222223</v>
+      </c>
+      <c r="B17">
+        <v>13.26</v>
+      </c>
+      <c r="C17">
+        <v>24.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1703,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,6 +1936,17 @@
         <v>25.4</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.408333333333</v>
+      </c>
+      <c r="B17">
+        <v>13.36</v>
+      </c>
+      <c r="C17">
+        <v>24.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1899,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2088,6 +2143,17 @@
         <v>21.6</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.422222222223</v>
+      </c>
+      <c r="B17">
+        <v>13.77</v>
+      </c>
+      <c r="C17">
+        <v>21.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2095,10 +2161,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2284,6 +2350,17 @@
         <v>18.600000000000001</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.429861111108</v>
+      </c>
+      <c r="B17">
+        <v>13.77</v>
+      </c>
+      <c r="C17">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2291,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2480,6 +2557,17 @@
         <v>23.6</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.461111111108</v>
+      </c>
+      <c r="B17">
+        <v>46.87</v>
+      </c>
+      <c r="C17">
+        <v>21.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2487,10 +2575,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2676,6 +2764,17 @@
         <v>25.5</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44054.45</v>
+      </c>
+      <c r="B17">
+        <v>223.08</v>
+      </c>
+      <c r="C17">
+        <v>22.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New data from sampling 8/26
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E4E184-44C9-4FE0-A9DA-5167BAB4BD65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96DDFBB-AD80-4389-851A-AD25205E6496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37800" yWindow="0" windowWidth="11100" windowHeight="15615" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,6 +947,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44069.387499999997</v>
+      </c>
+      <c r="B5">
+        <v>105.15</v>
+      </c>
+      <c r="C5">
+        <v>25.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -956,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5520A0B-2863-440F-B808-95ED3523429B}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -1125,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,6 +1336,17 @@
         <v>24.5</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.559027777781</v>
+      </c>
+      <c r="B18">
+        <v>12.43</v>
+      </c>
+      <c r="C18">
+        <v>27.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1333,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1533,6 +1555,17 @@
         <v>22.6</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.591666666667</v>
+      </c>
+      <c r="B18">
+        <v>42.22</v>
+      </c>
+      <c r="C18">
+        <v>24.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1540,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,6 +1773,17 @@
         <v>24.3</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.406944444447</v>
+      </c>
+      <c r="B18">
+        <v>10.18</v>
+      </c>
+      <c r="C18">
+        <v>25.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1747,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,6 +1991,17 @@
         <v>24.6</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.425000000003</v>
+      </c>
+      <c r="B18">
+        <v>13.74</v>
+      </c>
+      <c r="C18">
+        <v>26.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1954,10 +2009,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2154,6 +2209,17 @@
         <v>21.2</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.443055555559</v>
+      </c>
+      <c r="B18">
+        <v>11.52</v>
+      </c>
+      <c r="C18">
+        <v>22.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2161,10 +2227,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2361,6 +2427,17 @@
         <v>17.899999999999999</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.454861111109</v>
+      </c>
+      <c r="B18">
+        <v>9.76</v>
+      </c>
+      <c r="C18">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2368,10 +2445,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2568,6 +2645,17 @@
         <v>21.9</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.479861111111</v>
+      </c>
+      <c r="B18">
+        <v>42.68</v>
+      </c>
+      <c r="C18">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2575,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2775,6 +2863,17 @@
         <v>22.9</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44069.496527777781</v>
+      </c>
+      <c r="B18">
+        <v>327.63</v>
+      </c>
+      <c r="C18">
+        <v>24.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data from sampling today
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96DDFBB-AD80-4389-851A-AD25205E6496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D758E-FFB3-495B-8EA0-5CBAAE7BF137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37800" yWindow="0" windowWidth="11100" windowHeight="15615" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,6 +956,17 @@
       </c>
       <c r="C5">
         <v>25.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44082.375</v>
+      </c>
+      <c r="B6">
+        <v>46.65</v>
+      </c>
+      <c r="C6">
+        <v>17.3</v>
       </c>
     </row>
   </sheetData>
@@ -1136,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,6 +1358,17 @@
         <v>27.4</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.489583333336</v>
+      </c>
+      <c r="B19">
+        <v>469.9</v>
+      </c>
+      <c r="C19">
+        <v>17.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1355,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,6 +1588,17 @@
         <v>24.6</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.511805555558</v>
+      </c>
+      <c r="B19">
+        <v>132.59</v>
+      </c>
+      <c r="C19">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1573,10 +1606,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,6 +1817,17 @@
         <v>25.5</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.39166666667</v>
+      </c>
+      <c r="B19">
+        <v>43.71</v>
+      </c>
+      <c r="C19">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1791,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2002,6 +2046,17 @@
         <v>26.8</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.409722222219</v>
+      </c>
+      <c r="B19">
+        <v>35.83</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2009,10 +2064,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2220,6 +2275,17 @@
         <v>22.6</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.429166666669</v>
+      </c>
+      <c r="B19">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C19">
+        <v>14.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2227,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2438,6 +2504,17 @@
         <v>20.100000000000001</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.439583333333</v>
+      </c>
+      <c r="B19">
+        <v>15.66</v>
+      </c>
+      <c r="C19">
+        <v>12.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2445,10 +2522,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2656,6 +2733,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.45416666667</v>
+      </c>
+      <c r="B19">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2663,10 +2751,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2874,6 +2962,17 @@
         <v>24.7</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44082.463194444441</v>
+      </c>
+      <c r="B19">
+        <v>51.2</v>
+      </c>
+      <c r="C19">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
making good progress on salt routes. deal with w route 30 tomorrow
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\CL_BUD\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D758E-FFB3-495B-8EA0-5CBAAE7BF137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A03B6F-454D-42C6-B748-97D38031F8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="990" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -892,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -960,10 +960,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44082.375</v>
+        <v>44096.388888888891</v>
       </c>
       <c r="B6">
-        <v>46.65</v>
+        <v>37.35</v>
       </c>
       <c r="C6">
         <v>17.3</v>
@@ -1360,13 +1360,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.489583333336</v>
+        <v>44096.490972222222</v>
       </c>
       <c r="B19">
-        <v>469.9</v>
+        <v>12.06</v>
       </c>
       <c r="C19">
-        <v>17.8</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1590,13 +1590,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.511805555558</v>
+        <v>44096.511111111111</v>
       </c>
       <c r="B19">
-        <v>132.59</v>
+        <v>15.5</v>
       </c>
       <c r="C19">
-        <v>16.399999999999999</v>
+        <v>17.3</v>
       </c>
     </row>
   </sheetData>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.39166666667</v>
+        <v>44096.402777777781</v>
       </c>
       <c r="B19">
-        <v>43.71</v>
+        <v>10.82</v>
       </c>
       <c r="C19">
-        <v>18.600000000000001</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2048,13 +2048,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.409722222219</v>
+        <v>44096.418749999997</v>
       </c>
       <c r="B19">
-        <v>35.83</v>
+        <v>11.76</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2277,13 +2277,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.429166666669</v>
+        <v>44096.436111111114</v>
       </c>
       <c r="B19">
-        <v>19.399999999999999</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="C19">
-        <v>14.6</v>
+        <v>15.4</v>
       </c>
     </row>
   </sheetData>
@@ -2296,7 +2296,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,13 +2506,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.439583333333</v>
+        <v>44096.444444444445</v>
       </c>
       <c r="B19">
-        <v>15.66</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="C19">
-        <v>12.9</v>
+        <v>14.3</v>
       </c>
     </row>
   </sheetData>
@@ -2735,13 +2735,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.45416666667</v>
+        <v>44096.459722222222</v>
       </c>
       <c r="B19">
-        <v>81.099999999999994</v>
+        <v>39</v>
       </c>
       <c r="C19">
-        <v>16</v>
+        <v>16.7</v>
       </c>
     </row>
   </sheetData>
@@ -2753,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2964,13 +2964,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44082.463194444441</v>
+        <v>44096.468055555553</v>
       </c>
       <c r="B19">
-        <v>51.2</v>
+        <v>168.62</v>
       </c>
       <c r="C19">
-        <v>16.600000000000001</v>
+        <v>20.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data and working on model fit for river site linear regressions
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A03B6F-454D-42C6-B748-97D38031F8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E24FBFE-9031-40B9-BE9E-0AE597F1B438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="990" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29670" yWindow="4830" windowWidth="13830" windowHeight="7170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,6 +967,17 @@
       </c>
       <c r="C6">
         <v>17.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44110.361111111109</v>
+      </c>
+      <c r="B7">
+        <v>77.38</v>
+      </c>
+      <c r="C7">
+        <v>12.6</v>
       </c>
     </row>
   </sheetData>
@@ -1147,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,6 +1380,17 @@
         <v>19.600000000000001</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.461805555555</v>
+      </c>
+      <c r="B20">
+        <v>13.69</v>
+      </c>
+      <c r="C20">
+        <v>16.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1377,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,6 +1621,17 @@
         <v>17.3</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.481249999997</v>
+      </c>
+      <c r="B20">
+        <v>70.87</v>
+      </c>
+      <c r="C20">
+        <v>12.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1606,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,6 +1861,17 @@
         <v>18.100000000000001</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.375</v>
+      </c>
+      <c r="B20">
+        <v>18.96</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1835,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,6 +2101,17 @@
         <v>18.100000000000001</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.392361111109</v>
+      </c>
+      <c r="B20">
+        <v>14.65</v>
+      </c>
+      <c r="C20">
+        <v>11.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2064,10 +2119,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,6 +2341,17 @@
         <v>15.4</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.406944444447</v>
+      </c>
+      <c r="B20">
+        <v>17.46</v>
+      </c>
+      <c r="C20">
+        <v>11.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2293,10 +2359,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2515,6 +2581,17 @@
         <v>14.3</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.415277777778</v>
+      </c>
+      <c r="B20">
+        <v>10.36</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2522,10 +2599,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2744,6 +2821,17 @@
         <v>16.7</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.430555555555</v>
+      </c>
+      <c r="B20">
+        <v>45.38</v>
+      </c>
+      <c r="C20">
+        <v>12.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2751,10 +2839,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2973,6 +3061,17 @@
         <v>20.3</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44110.438888888886</v>
+      </c>
+      <c r="B20">
+        <v>356.07</v>
+      </c>
+      <c r="C20">
+        <v>15.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new data from field today
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E24FBFE-9031-40B9-BE9E-0AE597F1B438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BCBCF2-4C8E-41C4-AF60-C2299B627112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29670" yWindow="4830" windowWidth="13830" windowHeight="7170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-900" yWindow="564" windowWidth="17280" windowHeight="8976" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -890,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,6 +978,17 @@
       </c>
       <c r="C7">
         <v>12.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44134.444444444445</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>
@@ -1158,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,6 +1402,17 @@
         <v>16.2</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.479166666664</v>
+      </c>
+      <c r="B21">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>8.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1399,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,6 +1654,17 @@
         <v>12.6</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.525694444441</v>
+      </c>
+      <c r="B21">
+        <v>108</v>
+      </c>
+      <c r="C21">
+        <v>6.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1639,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,6 +1905,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.325694444444</v>
+      </c>
+      <c r="B21">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="C21">
+        <v>7.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1879,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2112,6 +2156,17 @@
         <v>11.8</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.345138888886</v>
+      </c>
+      <c r="B21">
+        <v>27.74</v>
+      </c>
+      <c r="C21">
+        <v>3.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2119,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,6 +2407,17 @@
         <v>11.1</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.35833333333</v>
+      </c>
+      <c r="B21">
+        <v>51.45</v>
+      </c>
+      <c r="C21">
+        <v>4.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2359,10 +2425,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2592,6 +2658,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.368055555555</v>
+      </c>
+      <c r="B21">
+        <v>51.6</v>
+      </c>
+      <c r="C21">
+        <v>4.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2599,10 +2676,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2832,6 +2909,17 @@
         <v>12.3</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.384027777778</v>
+      </c>
+      <c r="B21">
+        <v>134</v>
+      </c>
+      <c r="C21">
+        <v>5.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2839,10 +2927,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3072,6 +3160,17 @@
         <v>15.8</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44134.397222222222</v>
+      </c>
+      <c r="B21">
+        <v>288.2</v>
+      </c>
+      <c r="C21">
+        <v>5.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new data, continuing outlier work
</commit_message>
<xml_diff>
--- a/Data/chloride_field.xlsx
+++ b/Data/chloride_field.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linne\Box Sync\Chloride Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BCBCF2-4C8E-41C4-AF60-C2299B627112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7204B3-E1A4-45F3-8B88-89AFB4A8F8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-900" yWindow="564" windowWidth="17280" windowHeight="8976" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31635" yWindow="2970" windowWidth="17280" windowHeight="8970" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIC" sheetId="11" r:id="rId1"/>
@@ -54,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +185,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,10 +537,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -890,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170511C4-9B95-4BE9-8C35-7117D40D32CB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,10 +967,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44096.388888888891</v>
+        <v>44082.375</v>
       </c>
       <c r="B6">
-        <v>37.35</v>
+        <v>56.65</v>
       </c>
       <c r="C6">
         <v>17.3</v>
@@ -971,23 +978,34 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44110.361111111109</v>
+        <v>44096.388888888891</v>
       </c>
       <c r="B7">
-        <v>77.38</v>
+        <v>37.35</v>
       </c>
       <c r="C7">
-        <v>12.6</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <v>44110.361111111109</v>
+      </c>
+      <c r="B8">
+        <v>77.38</v>
+      </c>
+      <c r="C8">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>44134.444444444445</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>90</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>4.5</v>
       </c>
     </row>
@@ -1169,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,34 +1400,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.490972222222</v>
+        <v>44082.489583333336</v>
       </c>
       <c r="B19">
-        <v>12.06</v>
+        <v>58.99</v>
       </c>
       <c r="C19">
-        <v>19.600000000000001</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.461805555555</v>
+        <v>44096.490972222222</v>
       </c>
       <c r="B20">
-        <v>13.69</v>
+        <v>12.06</v>
       </c>
       <c r="C20">
-        <v>16.2</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.461805555555</v>
+      </c>
+      <c r="B21">
+        <v>13.69</v>
+      </c>
+      <c r="C21">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.479166666664</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>37</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>8.4</v>
       </c>
     </row>
@@ -1421,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,34 +1663,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.511111111111</v>
+        <v>44082.511805555558</v>
       </c>
       <c r="B19">
-        <v>15.5</v>
+        <v>132.59</v>
       </c>
       <c r="C19">
-        <v>17.3</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.481249999997</v>
+        <v>44096.511111111111</v>
       </c>
       <c r="B20">
-        <v>70.87</v>
+        <v>15.5</v>
       </c>
       <c r="C20">
-        <v>12.6</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.481249999997</v>
+      </c>
+      <c r="B21">
+        <v>70.87</v>
+      </c>
+      <c r="C21">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.525694444441</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>108</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>6.5</v>
       </c>
     </row>
@@ -1672,10 +1712,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,34 +1925,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.402777777781</v>
+        <v>44082.39166666667</v>
       </c>
       <c r="B19">
-        <v>10.82</v>
+        <v>43.71</v>
       </c>
       <c r="C19">
-        <v>18.100000000000001</v>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.375</v>
+        <v>44096.402777777781</v>
       </c>
       <c r="B20">
-        <v>18.96</v>
+        <v>10.82</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.375</v>
+      </c>
+      <c r="B21">
+        <v>18.96</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.325694444444</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>38.450000000000003</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>7.6</v>
       </c>
     </row>
@@ -1923,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2136,34 +2187,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.418749999997</v>
+        <v>44082.409722222219</v>
       </c>
       <c r="B19">
-        <v>11.76</v>
+        <v>35.83</v>
       </c>
       <c r="C19">
-        <v>18.100000000000001</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.392361111109</v>
+        <v>44096.418749999997</v>
       </c>
       <c r="B20">
-        <v>14.65</v>
+        <v>11.76</v>
       </c>
       <c r="C20">
-        <v>11.8</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.392361111109</v>
+      </c>
+      <c r="B21">
+        <v>14.65</v>
+      </c>
+      <c r="C21">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.345138888886</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>27.74</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>3.4</v>
       </c>
     </row>
@@ -2174,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2387,34 +2449,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.436111111114</v>
+        <v>44082.429166666669</v>
       </c>
       <c r="B19">
-        <v>10.039999999999999</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="C19">
-        <v>15.4</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.406944444447</v>
+        <v>44096.436111111114</v>
       </c>
       <c r="B20">
-        <v>17.46</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="C20">
-        <v>11.1</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.406944444447</v>
+      </c>
+      <c r="B21">
+        <v>17.46</v>
+      </c>
+      <c r="C21">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.35833333333</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>51.45</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>4.2</v>
       </c>
     </row>
@@ -2425,10 +2498,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2638,34 +2711,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.444444444445</v>
+        <v>44082.439583333333</v>
       </c>
       <c r="B19">
-        <v>8.8800000000000008</v>
+        <v>15.66</v>
       </c>
       <c r="C19">
-        <v>14.3</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.415277777778</v>
+        <v>44096.444444444445</v>
       </c>
       <c r="B20">
-        <v>10.36</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="C20">
-        <v>11</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.415277777778</v>
+      </c>
+      <c r="B21">
+        <v>10.36</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.368055555555</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>51.6</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>4.8</v>
       </c>
     </row>
@@ -2676,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2889,34 +2973,45 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44096.459722222222</v>
+        <v>44082.45416666667</v>
       </c>
       <c r="B19">
-        <v>39</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="C19">
-        <v>16.7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.430555555555</v>
+        <v>44096.459722222222</v>
       </c>
       <c r="B20">
-        <v>45.38</v>
+        <v>39</v>
       </c>
       <c r="C20">
-        <v>12.3</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.430555555555</v>
+      </c>
+      <c r="B21">
+        <v>45.38</v>
+      </c>
+      <c r="C21">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.384027777778</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>134</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>5.2</v>
       </c>
     </row>
@@ -2927,10 +3022,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3139,35 +3234,46 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>44096.468055555553</v>
+      <c r="A19" s="3">
+        <v>44082.463194444441</v>
       </c>
       <c r="B19">
-        <v>168.62</v>
+        <v>51.2</v>
       </c>
       <c r="C19">
-        <v>20.3</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44110.438888888886</v>
+        <v>44096.468055555553</v>
       </c>
       <c r="B20">
-        <v>356.07</v>
+        <v>168.62</v>
       </c>
       <c r="C20">
-        <v>15.8</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
+        <v>44110.438888888886</v>
+      </c>
+      <c r="B21">
+        <v>356.07</v>
+      </c>
+      <c r="C21">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>44134.397222222222</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>288.2</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>5.4</v>
       </c>
     </row>

</xml_diff>